<commit_message>
Adicionando inserção no banco de dados com loop por município e alterando logs
</commit_message>
<xml_diff>
--- a/OcorrenciaMensal(Criminal)-Cubatão_2025.xlsx
+++ b/OcorrenciaMensal(Criminal)-Cubatão_2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/guilherme_peres_sptech_school/Documents/sptech/Projeto PI - 2 Semestre/vigilante-backend/Base de dados/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/guilherme_peres_sptech_school/Documents/sptech/Projeto PI - 2 Semestre/vigilante-backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_9440F779D39F2ED7A71356AD04C7FF4EDC8DFA14" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BDA02E6-9791-4244-9D68-B1F4A1823AAF}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_9440F779D39F2ED7A71356AD04C7FF4EDC8DFA14" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD507A85-9A7D-4C24-BF5E-79042F407E2E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -343,10 +343,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -653,6 +649,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="58.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">

</xml_diff>